<commit_message>
Thay đổi câu trả lời
</commit_message>
<xml_diff>
--- a/Quiz1__Computer Fundamentals.xlsx
+++ b/Quiz1__Computer Fundamentals.xlsx
@@ -576,7 +576,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -637,25 +637,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -666,6 +647,28 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -918,8 +921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z971"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="L55" sqref="L55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -1083,10 +1086,10 @@
       <c r="A6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="27"/>
+      <c r="C6" s="36"/>
       <c r="D6" s="7"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -1112,13 +1115,13 @@
       <c r="Z6" s="1"/>
     </row>
     <row r="7" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="27"/>
+      <c r="C7" s="36"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -1144,7 +1147,7 @@
       <c r="Z7" s="1"/>
     </row>
     <row r="8" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A8" s="29"/>
+      <c r="A8" s="33"/>
       <c r="B8" s="8" t="s">
         <v>7</v>
       </c>
@@ -1176,7 +1179,7 @@
       <c r="Z8" s="1"/>
     </row>
     <row r="9" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A9" s="29"/>
+      <c r="A9" s="33"/>
       <c r="B9" s="8" t="s">
         <v>8</v>
       </c>
@@ -1208,7 +1211,7 @@
       <c r="Z9" s="1"/>
     </row>
     <row r="10" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A10" s="29"/>
+      <c r="A10" s="33"/>
       <c r="B10" s="8" t="s">
         <v>9</v>
       </c>
@@ -1240,14 +1243,14 @@
       <c r="Z10" s="1"/>
     </row>
     <row r="11" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A11" s="30"/>
+      <c r="A11" s="34"/>
       <c r="B11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="36">
+      <c r="C11" s="27">
         <v>7</v>
       </c>
-      <c r="D11" s="35" t="s">
+      <c r="D11" s="26" t="s">
         <v>85</v>
       </c>
       <c r="E11" s="1"/>
@@ -1274,13 +1277,13 @@
       <c r="Z11" s="1"/>
     </row>
     <row r="12" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="27"/>
+      <c r="C12" s="36"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -1306,7 +1309,7 @@
       <c r="Z12" s="1"/>
     </row>
     <row r="13" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A13" s="29"/>
+      <c r="A13" s="33"/>
       <c r="B13" s="8" t="s">
         <v>7</v>
       </c>
@@ -1338,14 +1341,14 @@
       <c r="Z13" s="1"/>
     </row>
     <row r="14" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A14" s="29"/>
+      <c r="A14" s="33"/>
       <c r="B14" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="36" t="s">
+      <c r="C14" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="35" t="s">
+      <c r="D14" s="26" t="s">
         <v>85</v>
       </c>
       <c r="E14" s="1"/>
@@ -1372,7 +1375,7 @@
       <c r="Z14" s="1"/>
     </row>
     <row r="15" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A15" s="29"/>
+      <c r="A15" s="33"/>
       <c r="B15" s="8" t="s">
         <v>9</v>
       </c>
@@ -1404,7 +1407,7 @@
       <c r="Z15" s="1"/>
     </row>
     <row r="16" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A16" s="30"/>
+      <c r="A16" s="34"/>
       <c r="B16" s="8" t="s">
         <v>10</v>
       </c>
@@ -1436,13 +1439,13 @@
       <c r="Z16" s="1"/>
     </row>
     <row r="17" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="27"/>
+      <c r="C17" s="36"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -1468,14 +1471,14 @@
       <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A18" s="29"/>
+      <c r="A18" s="33"/>
       <c r="B18" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="37" t="s">
+      <c r="C18" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="35" t="s">
+      <c r="D18" s="26" t="s">
         <v>85</v>
       </c>
       <c r="E18" s="1"/>
@@ -1502,7 +1505,7 @@
       <c r="Z18" s="1"/>
     </row>
     <row r="19" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A19" s="29"/>
+      <c r="A19" s="33"/>
       <c r="B19" s="8" t="s">
         <v>8</v>
       </c>
@@ -1534,7 +1537,7 @@
       <c r="Z19" s="1"/>
     </row>
     <row r="20" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A20" s="29"/>
+      <c r="A20" s="33"/>
       <c r="B20" s="8" t="s">
         <v>9</v>
       </c>
@@ -1566,7 +1569,7 @@
       <c r="Z20" s="1"/>
     </row>
     <row r="21" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A21" s="30"/>
+      <c r="A21" s="34"/>
       <c r="B21" s="8" t="s">
         <v>10</v>
       </c>
@@ -1598,13 +1601,13 @@
       <c r="Z21" s="1"/>
     </row>
     <row r="22" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A22" s="28" t="s">
+      <c r="A22" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="31" t="s">
+      <c r="B22" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="27"/>
+      <c r="C22" s="36"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -1630,14 +1633,14 @@
       <c r="Z22" s="1"/>
     </row>
     <row r="23" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A23" s="29"/>
+      <c r="A23" s="33"/>
       <c r="B23" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="38" t="s">
+      <c r="C23" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="35" t="s">
+      <c r="D23" s="26" t="s">
         <v>85</v>
       </c>
       <c r="E23" s="1"/>
@@ -1664,7 +1667,7 @@
       <c r="Z23" s="1"/>
     </row>
     <row r="24" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A24" s="29"/>
+      <c r="A24" s="33"/>
       <c r="B24" s="8" t="s">
         <v>8</v>
       </c>
@@ -1696,7 +1699,7 @@
       <c r="Z24" s="1"/>
     </row>
     <row r="25" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A25" s="29"/>
+      <c r="A25" s="33"/>
       <c r="B25" s="8" t="s">
         <v>9</v>
       </c>
@@ -1728,7 +1731,7 @@
       <c r="Z25" s="1"/>
     </row>
     <row r="26" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A26" s="30"/>
+      <c r="A26" s="34"/>
       <c r="B26" s="8" t="s">
         <v>10</v>
       </c>
@@ -1760,13 +1763,13 @@
       <c r="Z26" s="1"/>
     </row>
     <row r="27" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="31" t="s">
+      <c r="B27" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="27"/>
+      <c r="C27" s="36"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -1792,7 +1795,7 @@
       <c r="Z27" s="1"/>
     </row>
     <row r="28" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A28" s="29"/>
+      <c r="A28" s="33"/>
       <c r="B28" s="8" t="s">
         <v>7</v>
       </c>
@@ -1824,7 +1827,7 @@
       <c r="Z28" s="1"/>
     </row>
     <row r="29" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A29" s="29"/>
+      <c r="A29" s="33"/>
       <c r="B29" s="8" t="s">
         <v>8</v>
       </c>
@@ -1856,14 +1859,14 @@
       <c r="Z29" s="1"/>
     </row>
     <row r="30" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A30" s="29"/>
+      <c r="A30" s="33"/>
       <c r="B30" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C30" s="36" t="s">
+      <c r="C30" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="D30" s="35" t="s">
+      <c r="D30" s="26" t="s">
         <v>85</v>
       </c>
       <c r="E30" s="1"/>
@@ -1890,7 +1893,7 @@
       <c r="Z30" s="1"/>
     </row>
     <row r="31" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A31" s="30"/>
+      <c r="A31" s="34"/>
       <c r="B31" s="8" t="s">
         <v>10</v>
       </c>
@@ -1922,13 +1925,13 @@
       <c r="Z31" s="1"/>
     </row>
     <row r="32" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A32" s="28" t="s">
+      <c r="A32" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="31" t="s">
+      <c r="B32" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="C32" s="27"/>
+      <c r="C32" s="36"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -1954,7 +1957,7 @@
       <c r="Z32" s="1"/>
     </row>
     <row r="33" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A33" s="29"/>
+      <c r="A33" s="33"/>
       <c r="B33" s="8" t="s">
         <v>7</v>
       </c>
@@ -1986,7 +1989,7 @@
       <c r="Z33" s="1"/>
     </row>
     <row r="34" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A34" s="29"/>
+      <c r="A34" s="33"/>
       <c r="B34" s="8" t="s">
         <v>8</v>
       </c>
@@ -2018,14 +2021,14 @@
       <c r="Z34" s="1"/>
     </row>
     <row r="35" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A35" s="29"/>
+      <c r="A35" s="33"/>
       <c r="B35" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="36" t="s">
+      <c r="C35" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="D35" s="35" t="s">
+      <c r="D35" s="26" t="s">
         <v>85</v>
       </c>
       <c r="E35" s="1"/>
@@ -2052,7 +2055,7 @@
       <c r="Z35" s="1"/>
     </row>
     <row r="36" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A36" s="30"/>
+      <c r="A36" s="34"/>
       <c r="B36" s="8" t="s">
         <v>10</v>
       </c>
@@ -2084,13 +2087,13 @@
       <c r="Z36" s="1"/>
     </row>
     <row r="37" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A37" s="28" t="s">
+      <c r="A37" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="B37" s="33" t="s">
+      <c r="B37" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="34"/>
+      <c r="C37" s="39"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -2116,7 +2119,7 @@
       <c r="Z37" s="1"/>
     </row>
     <row r="38" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A38" s="29"/>
+      <c r="A38" s="33"/>
       <c r="B38" s="8" t="s">
         <v>7</v>
       </c>
@@ -2148,7 +2151,7 @@
       <c r="Z38" s="1"/>
     </row>
     <row r="39" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A39" s="29"/>
+      <c r="A39" s="33"/>
       <c r="B39" s="8" t="s">
         <v>8</v>
       </c>
@@ -2180,7 +2183,7 @@
       <c r="Z39" s="1"/>
     </row>
     <row r="40" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A40" s="29"/>
+      <c r="A40" s="33"/>
       <c r="B40" s="8" t="s">
         <v>9</v>
       </c>
@@ -2212,11 +2215,11 @@
       <c r="Z40" s="1"/>
     </row>
     <row r="41" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A41" s="30"/>
+      <c r="A41" s="34"/>
       <c r="B41" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C41" s="39" t="s">
+      <c r="C41" s="30" t="s">
         <v>46</v>
       </c>
       <c r="D41" s="1"/>
@@ -2244,13 +2247,13 @@
       <c r="Z41" s="1"/>
     </row>
     <row r="42" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A42" s="28" t="s">
+      <c r="A42" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="B42" s="31" t="s">
+      <c r="B42" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="C42" s="27"/>
+      <c r="C42" s="36"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
@@ -2276,7 +2279,7 @@
       <c r="Z42" s="1"/>
     </row>
     <row r="43" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A43" s="29"/>
+      <c r="A43" s="33"/>
       <c r="B43" s="8" t="s">
         <v>7</v>
       </c>
@@ -2308,11 +2311,11 @@
       <c r="Z43" s="1"/>
     </row>
     <row r="44" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A44" s="29"/>
+      <c r="A44" s="33"/>
       <c r="B44" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C44" s="36" t="s">
+      <c r="C44" s="27" t="s">
         <v>50</v>
       </c>
       <c r="D44" s="1"/>
@@ -2340,7 +2343,7 @@
       <c r="Z44" s="1"/>
     </row>
     <row r="45" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A45" s="29"/>
+      <c r="A45" s="33"/>
       <c r="B45" s="8" t="s">
         <v>9</v>
       </c>
@@ -2372,7 +2375,7 @@
       <c r="Z45" s="1"/>
     </row>
     <row r="46" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A46" s="30"/>
+      <c r="A46" s="34"/>
       <c r="B46" s="8" t="s">
         <v>10</v>
       </c>
@@ -2404,13 +2407,13 @@
       <c r="Z46" s="1"/>
     </row>
     <row r="47" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A47" s="28" t="s">
+      <c r="A47" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="B47" s="32" t="s">
+      <c r="B47" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="C47" s="27"/>
+      <c r="C47" s="36"/>
       <c r="D47" s="13"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
@@ -2436,7 +2439,7 @@
       <c r="Z47" s="1"/>
     </row>
     <row r="48" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A48" s="29"/>
+      <c r="A48" s="33"/>
       <c r="B48" s="14" t="s">
         <v>7</v>
       </c>
@@ -2468,11 +2471,11 @@
       <c r="Z48" s="1"/>
     </row>
     <row r="49" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A49" s="29"/>
+      <c r="A49" s="33"/>
       <c r="B49" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C49" s="40" t="s">
+      <c r="C49" s="41" t="s">
         <v>56</v>
       </c>
       <c r="D49" s="1"/>
@@ -2500,7 +2503,7 @@
       <c r="Z49" s="1"/>
     </row>
     <row r="50" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A50" s="29"/>
+      <c r="A50" s="33"/>
       <c r="B50" s="14" t="s">
         <v>9</v>
       </c>
@@ -2532,11 +2535,11 @@
       <c r="Z50" s="1"/>
     </row>
     <row r="51" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A51" s="30"/>
+      <c r="A51" s="34"/>
       <c r="B51" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C51" s="15" t="s">
+      <c r="C51" s="31" t="s">
         <v>58</v>
       </c>
       <c r="D51" s="1"/>
@@ -2564,13 +2567,13 @@
       <c r="Z51" s="1"/>
     </row>
     <row r="52" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A52" s="28" t="s">
+      <c r="A52" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="B52" s="31" t="s">
+      <c r="B52" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="C52" s="27"/>
+      <c r="C52" s="36"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
@@ -2596,7 +2599,7 @@
       <c r="Z52" s="1"/>
     </row>
     <row r="53" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A53" s="29"/>
+      <c r="A53" s="33"/>
       <c r="B53" s="8" t="s">
         <v>7</v>
       </c>
@@ -2628,7 +2631,7 @@
       <c r="Z53" s="1"/>
     </row>
     <row r="54" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A54" s="29"/>
+      <c r="A54" s="33"/>
       <c r="B54" s="8" t="s">
         <v>8</v>
       </c>
@@ -2660,7 +2663,7 @@
       <c r="Z54" s="1"/>
     </row>
     <row r="55" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A55" s="29"/>
+      <c r="A55" s="33"/>
       <c r="B55" s="8" t="s">
         <v>9</v>
       </c>
@@ -2692,11 +2695,11 @@
       <c r="Z55" s="1"/>
     </row>
     <row r="56" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A56" s="30"/>
+      <c r="A56" s="34"/>
       <c r="B56" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C56" s="36" t="s">
+      <c r="C56" s="27" t="s">
         <v>64</v>
       </c>
       <c r="D56" s="1"/>
@@ -28345,6 +28348,16 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="A37:A41"/>
+    <mergeCell ref="A42:A46"/>
+    <mergeCell ref="A47:A51"/>
     <mergeCell ref="A52:A56"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="B47:C47"/>
@@ -28356,16 +28369,6 @@
     <mergeCell ref="A32:A36"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="B37:C37"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="A37:A41"/>
-    <mergeCell ref="A42:A46"/>
-    <mergeCell ref="A47:A51"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <phoneticPr fontId="13"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>